<commit_message>
New results for experiments with meta-features
</commit_message>
<xml_diff>
--- a/results/bipop-results-ntries30-searchspace0.1.xlsx
+++ b/results/bipop-results-ntries30-searchspace0.1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="19">
   <si>
     <t>dataset</t>
   </si>
@@ -34,49 +34,40 @@
     <t>search_space</t>
   </si>
   <si>
-    <t>100_features_0.1_error.csv</t>
-  </si>
-  <si>
-    <t>10_features_0.1_error.csv</t>
-  </si>
-  <si>
-    <t>5_features_0.01_error.csv</t>
-  </si>
-  <si>
-    <t>10_features_0.01_error.csv</t>
-  </si>
-  <si>
-    <t>5_features_0.1_error.csv</t>
-  </si>
-  <si>
-    <t>2_features_0.01_error.csv</t>
-  </si>
-  <si>
-    <t>2_features_0.1_error.csv</t>
-  </si>
-  <si>
-    <t>10_features_0.5_error.csv</t>
-  </si>
-  <si>
-    <t>100_features_0.5_error.csv</t>
-  </si>
-  <si>
-    <t>5_features_0.5_error.csv</t>
-  </si>
-  <si>
-    <t>2_features_0.5_error.csv</t>
-  </si>
-  <si>
-    <t>100_features_0.01_error.csv</t>
-  </si>
-  <si>
-    <t>credit-g_metadata.csv</t>
-  </si>
-  <si>
-    <t>compas_metadata.csv</t>
-  </si>
-  <si>
-    <t>XOR_metadata.csv</t>
+    <t>10_features_0.01_error.csv.csv</t>
+  </si>
+  <si>
+    <t>5_features_0.01_error.csv.csv</t>
+  </si>
+  <si>
+    <t>10_features_0.5_error.csv.csv</t>
+  </si>
+  <si>
+    <t>10_features_0.1_error.csv.csv</t>
+  </si>
+  <si>
+    <t>100_features_0.1_error.csv.csv</t>
+  </si>
+  <si>
+    <t>100_features_0.5_error.csv.csv</t>
+  </si>
+  <si>
+    <t>5_features_0.5_error.csv.csv</t>
+  </si>
+  <si>
+    <t>100_features_0.01_error.csv.csv</t>
+  </si>
+  <si>
+    <t>5_features_0.1_error.csv.csv</t>
+  </si>
+  <si>
+    <t>2_features_0.01_error.csv.csv</t>
+  </si>
+  <si>
+    <t>2_features_0.1_error.csv.csv</t>
+  </si>
+  <si>
+    <t>2_features_0.5_error.csv.csv</t>
   </si>
   <si>
     <t>bipop</t>
@@ -437,7 +428,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -471,13 +462,13 @@
         <v>6</v>
       </c>
       <c r="C2">
-        <v>35283.78252306203</v>
+        <v>7854.974847266059</v>
       </c>
       <c r="D2">
-        <v>153.8181040287018</v>
+        <v>2.539521217346191</v>
       </c>
       <c r="E2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F2">
         <v>30</v>
@@ -494,13 +485,13 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>944.0294755138837</v>
+        <v>7384.869514808409</v>
       </c>
       <c r="D3">
-        <v>2.117284059524536</v>
+        <v>2.529790163040161</v>
       </c>
       <c r="E3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F3">
         <v>30</v>
@@ -517,13 +508,13 @@
         <v>8</v>
       </c>
       <c r="C4">
-        <v>631.7612323623331</v>
+        <v>9075.575259189287</v>
       </c>
       <c r="D4">
-        <v>1.105007648468018</v>
+        <v>2.983652114868164</v>
       </c>
       <c r="E4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F4">
         <v>30</v>
@@ -540,13 +531,13 @@
         <v>9</v>
       </c>
       <c r="C5">
-        <v>943.882946965133</v>
+        <v>8225.308119585436</v>
       </c>
       <c r="D5">
-        <v>1.768929004669189</v>
+        <v>3.23308801651001</v>
       </c>
       <c r="E5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F5">
         <v>30</v>
@@ -563,13 +554,13 @@
         <v>10</v>
       </c>
       <c r="C6">
-        <v>622.8512539280075</v>
+        <v>7997.539347149157</v>
       </c>
       <c r="D6">
-        <v>1.094934225082397</v>
+        <v>3.222321748733521</v>
       </c>
       <c r="E6" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F6">
         <v>30</v>
@@ -586,13 +577,13 @@
         <v>11</v>
       </c>
       <c r="C7">
-        <v>539.1979833458479</v>
+        <v>9014.655831042939</v>
       </c>
       <c r="D7">
-        <v>0.4324700832366943</v>
+        <v>2.663567066192627</v>
       </c>
       <c r="E7" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F7">
         <v>30</v>
@@ -609,13 +600,13 @@
         <v>12</v>
       </c>
       <c r="C8">
-        <v>537.4572529758689</v>
+        <v>9310.509594784353</v>
       </c>
       <c r="D8">
-        <v>0.7086830139160156</v>
+        <v>2.627505779266357</v>
       </c>
       <c r="E8" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F8">
         <v>30</v>
@@ -632,13 +623,13 @@
         <v>13</v>
       </c>
       <c r="C9">
-        <v>938.1813741028714</v>
+        <v>8046.293624039642</v>
       </c>
       <c r="D9">
-        <v>2.145537137985229</v>
+        <v>2.640698909759521</v>
       </c>
       <c r="E9" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F9">
         <v>30</v>
@@ -655,13 +646,13 @@
         <v>14</v>
       </c>
       <c r="C10">
-        <v>35290.05595830352</v>
+        <v>8224.794069499589</v>
       </c>
       <c r="D10">
-        <v>143.5899729728699</v>
+        <v>2.661087989807129</v>
       </c>
       <c r="E10" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F10">
         <v>30</v>
@@ -678,13 +669,13 @@
         <v>15</v>
       </c>
       <c r="C11">
-        <v>593.8218835382053</v>
+        <v>7309.910203919307</v>
       </c>
       <c r="D11">
-        <v>1.326498031616211</v>
+        <v>3.539085865020752</v>
       </c>
       <c r="E11" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F11">
         <v>30</v>
@@ -701,13 +692,13 @@
         <v>16</v>
       </c>
       <c r="C12">
-        <v>542.2906454032047</v>
+        <v>8609.001889490926</v>
       </c>
       <c r="D12">
-        <v>0.441925048828125</v>
+        <v>2.680201768875122</v>
       </c>
       <c r="E12" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F12">
         <v>30</v>
@@ -724,87 +715,18 @@
         <v>17</v>
       </c>
       <c r="C13">
-        <v>35325.61544321163</v>
+        <v>9812.223000884836</v>
       </c>
       <c r="D13">
-        <v>155.2868740558624</v>
+        <v>2.807796955108643</v>
       </c>
       <c r="E13" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F13">
         <v>30</v>
       </c>
       <c r="G13">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="A14" s="1">
-        <v>12</v>
-      </c>
-      <c r="B14" t="s">
-        <v>18</v>
-      </c>
-      <c r="C14">
-        <v>11706.01524782877</v>
-      </c>
-      <c r="D14">
-        <v>2.450988054275513</v>
-      </c>
-      <c r="E14" t="s">
-        <v>21</v>
-      </c>
-      <c r="F14">
-        <v>30</v>
-      </c>
-      <c r="G14">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="A15" s="1">
-        <v>13</v>
-      </c>
-      <c r="B15" t="s">
-        <v>19</v>
-      </c>
-      <c r="C15">
-        <v>31440.89293689913</v>
-      </c>
-      <c r="D15">
-        <v>11.31266522407532</v>
-      </c>
-      <c r="E15" t="s">
-        <v>21</v>
-      </c>
-      <c r="F15">
-        <v>30</v>
-      </c>
-      <c r="G15">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="A16" s="1">
-        <v>14</v>
-      </c>
-      <c r="B16" t="s">
-        <v>20</v>
-      </c>
-      <c r="C16">
-        <v>5257.545444070401</v>
-      </c>
-      <c r="D16">
-        <v>2.434091806411743</v>
-      </c>
-      <c r="E16" t="s">
-        <v>21</v>
-      </c>
-      <c r="F16">
-        <v>30</v>
-      </c>
-      <c r="G16">
         <v>0.1</v>
       </c>
     </row>

</xml_diff>